<commit_message>
arif - test 2
</commit_message>
<xml_diff>
--- a/test_sipp_parallel.xlsx
+++ b/test_sipp_parallel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\05211740000055\Documents\UiPath\sippfirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C98A434-6503-41B0-AFA0-A7A8DDA24B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7845651D-295C-4944-85F8-1545BDC71D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" xr2:uid="{B39386CE-8DD5-429B-AD3F-000B5553CD9A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>sipp</t>
   </si>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026466D5-3DEF-4D09-B5AD-A099EB70171B}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A6:A15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,6 +434,46 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
To do (arif) - create temporary output for every link PN
</commit_message>
<xml_diff>
--- a/test_sipp_parallel.xlsx
+++ b/test_sipp_parallel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\05211740000055\Documents\UiPath\sippfirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7845651D-295C-4944-85F8-1545BDC71D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0528384A-B0B7-4F9A-82F1-4E98C3A9DC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" xr2:uid="{B39386CE-8DD5-429B-AD3F-000B5553CD9A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B39386CE-8DD5-429B-AD3F-000B5553CD9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>sipp</t>
   </si>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026466D5-3DEF-4D09-B5AD-A099EB70171B}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,46 +434,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>